<commit_message>
added new code examples & java8 material
</commit_message>
<xml_diff>
--- a/java8_material/functional_interfaces_java8.xlsx
+++ b/java8_material/functional_interfaces_java8.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>java.util.function</t>
   </si>
@@ -24,33 +24,15 @@
     <t>Functional Interface Name</t>
   </si>
   <si>
-    <t>Abstract Method Name</t>
-  </si>
-  <si>
-    <t>void accept(T t)</t>
-  </si>
-  <si>
-    <t>boolean test(T t)</t>
-  </si>
-  <si>
     <t>Predicate&lt;T&gt;</t>
   </si>
   <si>
     <t>BiConsumer&lt;K, V&gt;</t>
   </si>
   <si>
-    <t>void accept(K key, V value)</t>
-  </si>
-  <si>
     <t>Sr. No.</t>
   </si>
   <si>
-    <t>void run( )</t>
-  </si>
-  <si>
-    <t>T call( )</t>
-  </si>
-  <si>
     <t>Runnable&lt;&gt;</t>
   </si>
   <si>
@@ -63,20 +45,53 @@
     <t>Function&lt;R, T&gt;</t>
   </si>
   <si>
-    <t>R apply(T t)</t>
-  </si>
-  <si>
     <t>BiFunction&lt;R, T, U&gt;</t>
   </si>
   <si>
-    <t>R apply(T t, U u)</t>
+    <t xml:space="preserve">void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean </t>
+  </si>
+  <si>
+    <t xml:space="preserve">T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R </t>
+  </si>
+  <si>
+    <t>Return Type</t>
+  </si>
+  <si>
+    <t>Method Name</t>
+  </si>
+  <si>
+    <t>accept (T t)</t>
+  </si>
+  <si>
+    <t>accept (K key, V value)</t>
+  </si>
+  <si>
+    <t>test (T t)</t>
+  </si>
+  <si>
+    <t>run ( )</t>
+  </si>
+  <si>
+    <t>call ( )</t>
+  </si>
+  <si>
+    <t>apply (T t)</t>
+  </si>
+  <si>
+    <t>apply (T t, U u)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +109,13 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -206,23 +228,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,188 +560,225 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D21"/>
+  <dimension ref="B1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:5">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1">
+    <row r="2" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:5" ht="19.5" thickBot="1">
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="18.75">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="18.75">
+      <c r="B5" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="18.75">
+      <c r="B6" s="10">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="18.75">
+      <c r="B7" s="10">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="18.75">
+      <c r="B8" s="10">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="18.75">
+      <c r="B9" s="10">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="8">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="E9" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="18.75">
+      <c r="B10" s="10">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="8">
-        <v>3</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="8">
-        <v>4</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="18.75">
+      <c r="B11" s="10">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="2:5" ht="18.75">
+      <c r="B12" s="10">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="2:5" ht="18.75">
+      <c r="B13" s="10">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="2:5" ht="18.75">
+      <c r="B14" s="10">
         <v>11</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="8">
-        <v>5</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="2:5" ht="18.75">
+      <c r="B15" s="10">
         <v>12</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="8">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="2:5" ht="18.75">
+      <c r="B16" s="10">
+        <v>13</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="2:5" ht="18.75">
+      <c r="B17" s="10">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="2:5" ht="18.75">
+      <c r="B18" s="10">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="8">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="2:5" ht="18.75">
+      <c r="B19" s="10">
         <v>16</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="2:5" ht="18.75">
+      <c r="B20" s="10">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="8">
-        <v>8</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="8">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="8">
-        <v>10</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="8">
-        <v>11</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="8">
-        <v>12</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="8">
-        <v>13</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="8">
-        <v>14</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="8">
-        <v>15</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="8">
-        <v>16</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="8">
-        <v>17</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B21" s="10">
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B21" s="11">
         <v>18</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added Supplier FI to excell
</commit_message>
<xml_diff>
--- a/java8_material/functional_interfaces_java8.xlsx
+++ b/java8_material/functional_interfaces_java8.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>java.util.function</t>
   </si>
@@ -24,24 +24,12 @@
     <t>Functional Interface Name</t>
   </si>
   <si>
-    <t>Predicate&lt;T&gt;</t>
-  </si>
-  <si>
     <t>BiConsumer&lt;K, V&gt;</t>
   </si>
   <si>
     <t>Sr. No.</t>
   </si>
   <si>
-    <t>Runnable&lt;&gt;</t>
-  </si>
-  <si>
-    <t>Callable&lt;T&gt;</t>
-  </si>
-  <si>
-    <t>Consumer&lt;T t&gt;</t>
-  </si>
-  <si>
     <t>Function&lt;R, T&gt;</t>
   </si>
   <si>
@@ -85,6 +73,24 @@
   </si>
   <si>
     <t>apply (T t, U u)</t>
+  </si>
+  <si>
+    <t>get( )</t>
+  </si>
+  <si>
+    <t>Supplier&lt; T &gt;</t>
+  </si>
+  <si>
+    <t>Consumer&lt; T &gt;</t>
+  </si>
+  <si>
+    <t>Predicate&lt; T &gt;</t>
+  </si>
+  <si>
+    <t>Runnable&lt; &gt;</t>
+  </si>
+  <si>
+    <t>Callable&lt; T &gt;</t>
   </si>
 </sst>
 </file>
@@ -563,7 +569,7 @@
   <dimension ref="B1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -582,16 +588,16 @@
     <row r="2" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:5" ht="19.5" thickBot="1">
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="18.75">
@@ -599,13 +605,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="18.75">
@@ -613,13 +619,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75">
@@ -627,13 +633,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75">
@@ -641,13 +647,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75">
@@ -655,13 +661,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75">
@@ -669,13 +675,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="18.75">
@@ -683,22 +689,28 @@
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="18.75">
       <c r="B11" s="10">
         <v>8</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
+      <c r="C11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="2:5" ht="18.75">
       <c r="B12" s="10">

</xml_diff>